<commit_message>
step 2.1: intraday data
</commit_message>
<xml_diff>
--- a/xltrailtestbook.xlsx
+++ b/xltrailtestbook.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron Klopp\Documents\GitHub\mltools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benn/stuff/github/mltools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA68B1-8F80-479F-8225-755F5CE23894}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BD9EF4-EF25-594C-8F84-3AD61FD12498}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28035" windowHeight="17445" xr2:uid="{DC867D0E-7ED6-AA45-A55B-C097B6C59CBA}"/>
+    <workbookView xWindow="5900" yWindow="4120" windowWidth="28040" windowHeight="17440" xr2:uid="{DC867D0E-7ED6-AA45-A55B-C097B6C59CBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>Col1</t>
   </si>
@@ -96,9 +90,6 @@
     <t>hgfd</t>
   </si>
   <si>
-    <t>dgf</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -112,6 +103,36 @@
   </si>
   <si>
     <t>NEW</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>cow</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>fly</t>
   </si>
 </sst>
 </file>
@@ -160,18 +181,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -187,8 +211,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4AA0F90-DA58-8542-9B46-55E8C418B7B0}" name="Table1" displayName="Table1" ref="A1:F23" totalsRowShown="0">
-  <autoFilter ref="A1:F23" xr:uid="{2B1769B5-4172-314C-AC17-DCB565DCE055}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4AA0F90-DA58-8542-9B46-55E8C418B7B0}" name="Table1" displayName="Table1" ref="A1:F27" totalsRowShown="0">
+  <autoFilter ref="A1:F27" xr:uid="{2B1769B5-4172-314C-AC17-DCB565DCE055}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{556A75C3-EF4F-0A45-9C50-3542DEBDABD0}" name="Col1"/>
     <tableColumn id="2" xr3:uid="{2A60FE47-63B5-0248-9472-7C9E8D9CBE69}" name="Col2"/>
@@ -500,15 +524,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E5DF-D5F3-6F49-9652-E8184A481860}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,16 +543,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -536,20 +560,17 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <f>A2*D2</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -557,20 +578,20 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E23" si="0">A3*D3</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -578,20 +599,20 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -599,20 +620,20 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -620,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -630,10 +651,10 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -641,7 +662,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>5556</v>
@@ -651,10 +672,10 @@
         <v>16668</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -662,20 +683,20 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -683,20 +704,17 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -704,20 +722,20 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>176</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -725,7 +743,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>455</v>
@@ -735,10 +753,10 @@
         <v>1820</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -746,7 +764,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>456</v>
@@ -756,10 +774,10 @@
         <v>2280</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -767,7 +785,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>456</v>
@@ -777,10 +795,10 @@
         <v>1824</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>333</v>
       </c>
@@ -788,7 +806,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>56</v>
@@ -797,10 +815,10 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -808,20 +826,20 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>7655</v>
       </c>
       <c r="E15">
         <f>A4*E3</f>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -829,7 +847,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16">
         <v>68</v>
@@ -839,10 +857,10 @@
         <v>204</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>455</v>
       </c>
@@ -850,7 +868,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>67</v>
@@ -860,10 +878,10 @@
         <v>30485</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
@@ -871,7 +889,7 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18">
         <v>74</v>
@@ -881,10 +899,10 @@
         <v>370</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
@@ -892,7 +910,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19">
         <v>56</v>
@@ -902,10 +920,10 @@
         <v>224</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3455</v>
       </c>
@@ -913,7 +931,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20">
         <v>5346</v>
@@ -923,10 +941,10 @@
         <v>18470430</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
@@ -934,7 +952,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21">
         <v>674</v>
@@ -944,10 +962,10 @@
         <v>4044</v>
       </c>
       <c r="F21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -955,7 +973,7 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22">
         <v>5345</v>
@@ -965,28 +983,112 @@
         <v>21380</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E27" si="1">A24*D24</f>
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>10.1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>30.299999999999997</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>11.2</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>33.599999999999994</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
step 2.2: intraday data
</commit_message>
<xml_diff>
--- a/xltrailtestbook.xlsx
+++ b/xltrailtestbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benn/stuff/github/mltools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BD9EF4-EF25-594C-8F84-3AD61FD12498}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987ADA18-921F-9E45-8D9D-D1A228AA45C9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="4120" windowWidth="28040" windowHeight="17440" xr2:uid="{DC867D0E-7ED6-AA45-A55B-C097B6C59CBA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Col1</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Col3</t>
   </si>
   <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>gs</t>
-  </si>
-  <si>
     <t>dsf</t>
   </si>
   <si>
@@ -133,6 +127,18 @@
   </si>
   <si>
     <t>fly</t>
+  </si>
+  <si>
+    <t>v2.2</t>
+  </si>
+  <si>
+    <t>yup</t>
+  </si>
+  <si>
+    <t>lastrow</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -211,8 +217,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4AA0F90-DA58-8542-9B46-55E8C418B7B0}" name="Table1" displayName="Table1" ref="A1:F27" totalsRowShown="0">
-  <autoFilter ref="A1:F27" xr:uid="{2B1769B5-4172-314C-AC17-DCB565DCE055}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4AA0F90-DA58-8542-9B46-55E8C418B7B0}" name="Table1" displayName="Table1" ref="A1:F28" totalsRowShown="0">
+  <autoFilter ref="A1:F28" xr:uid="{2B1769B5-4172-314C-AC17-DCB565DCE055}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{556A75C3-EF4F-0A45-9C50-3542DEBDABD0}" name="Col1"/>
     <tableColumn id="2" xr3:uid="{2A60FE47-63B5-0248-9472-7C9E8D9CBE69}" name="Col2"/>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E5DF-D5F3-6F49-9652-E8184A481860}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,13 +549,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -557,17 +563,17 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <f>A2*D2</f>
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -575,10 +581,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -588,7 +594,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -596,10 +602,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -609,7 +615,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -617,10 +623,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -630,7 +636,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -638,10 +644,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -651,7 +657,7 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -659,10 +665,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>5556</v>
@@ -672,7 +678,7 @@
         <v>16668</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -680,10 +686,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -693,7 +699,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -701,10 +707,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>12</v>
@@ -719,10 +725,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -732,7 +738,7 @@
         <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -740,10 +746,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>455</v>
@@ -753,7 +759,7 @@
         <v>1820</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -761,10 +767,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12">
         <v>456</v>
@@ -774,7 +780,7 @@
         <v>2280</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -782,10 +788,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13">
         <v>456</v>
@@ -795,7 +801,7 @@
         <v>1824</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -803,10 +809,10 @@
         <v>333</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <v>56</v>
@@ -815,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -823,10 +829,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15">
         <v>7655</v>
@@ -836,7 +842,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -844,10 +850,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16">
         <v>68</v>
@@ -857,7 +863,7 @@
         <v>204</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -865,10 +871,10 @@
         <v>455</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D17">
         <v>67</v>
@@ -878,7 +884,7 @@
         <v>30485</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -886,10 +892,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>74</v>
@@ -899,7 +905,7 @@
         <v>370</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -907,10 +913,10 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19">
         <v>56</v>
@@ -920,7 +926,7 @@
         <v>224</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -928,10 +934,10 @@
         <v>3455</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D20">
         <v>5346</v>
@@ -941,7 +947,7 @@
         <v>18470430</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -949,10 +955,10 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21">
         <v>674</v>
@@ -962,7 +968,7 @@
         <v>4044</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -970,10 +976,10 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D22">
         <v>5345</v>
@@ -983,7 +989,7 @@
         <v>21380</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -991,10 +997,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23">
         <v>8</v>
@@ -1004,7 +1010,7 @@
         <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1012,10 +1018,10 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D24">
         <v>9</v>
@@ -1025,7 +1031,7 @@
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1033,10 +1039,10 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D25">
         <v>10.1</v>
@@ -1046,7 +1052,7 @@
         <v>30.299999999999997</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1054,10 +1060,10 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D26">
         <v>11.2</v>
@@ -1067,7 +1073,7 @@
         <v>33.599999999999994</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1075,10 +1081,10 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D27" s="3">
         <v>3</v>
@@ -1088,7 +1094,25 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>-3.3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ref="E28" si="2">A28*D28</f>
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
step 4: final changes of the day
</commit_message>
<xml_diff>
--- a/xltrailtestbook.xlsx
+++ b/xltrailtestbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benn/stuff/github/mltools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987ADA18-921F-9E45-8D9D-D1A228AA45C9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F49E828-F50B-DD40-BC9E-858228CCF9B9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="4120" windowWidth="28040" windowHeight="17440" xr2:uid="{DC867D0E-7ED6-AA45-A55B-C097B6C59CBA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
   <si>
     <t>Col1</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>highlight</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>conditional formatting</t>
   </si>
 </sst>
 </file>
@@ -148,7 +157,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,8 +172,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +191,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,18 +215,31 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -533,10 +569,13 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -559,42 +598,43 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="4">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4">
         <f>A2*D2</f>
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>23</v>
+      <c r="F2" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <f t="shared" ref="E3:E23" si="0">A3*D3</f>
         <v>4</v>
       </c>
-      <c r="F3" t="s">
-        <v>23</v>
+      <c r="F3" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -615,7 +655,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1116,6 +1156,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A4:F4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A$4&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>